<commit_message>
Se agrega uso de ventanas, se soluciona reto de CRM, entre otras
</commit_message>
<xml_diff>
--- a/build/resources/test/datadriven/registroLibros.xlsx
+++ b/build/resources/test/datadriven/registroLibros.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Selenium Ruby</t>
   </si>
@@ -33,6 +33,24 @@
   </si>
   <si>
     <t>Mastering JavaScript</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>My Account</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>AT Site</t>
+  </si>
+  <si>
+    <t>Demo Site</t>
+  </si>
+  <si>
+    <t>0 Items₹0.00</t>
   </si>
 </sst>
 </file>
@@ -351,28 +369,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>